<commit_message>
Updated Invoke workflow paths
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testb\Documents\UiPath\FederalBotFactory\TreasuryConfirmation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4684397E-B22A-4EC8-AEFD-4953805489F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF869B-CFE4-490C-91F0-CBE27FC69CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="279">
   <si>
     <t>Name</t>
   </si>
@@ -857,13 +857,10 @@
     <t>in number</t>
   </si>
   <si>
-    <t>gmahesh2789@gmail.com; hariharangouri@gmail.com</t>
-  </si>
-  <si>
-    <t>gmahesh2789@gmail.com; hariharangouri@gmail.com; sunil.melam@gmail.com</t>
-  </si>
-  <si>
     <t>TreasuryConfirmation_</t>
+  </si>
+  <si>
+    <t>testbotforuipath@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1079"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1566,7 +1563,7 @@
         <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1">
@@ -2347,7 +2344,7 @@
         <v>135</v>
       </c>
       <c r="B145" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C145" t="s">
         <v>45</v>

</xml_diff>